<commit_message>
Sexto commit - Finalización del grupo de factibles inmediatos
</commit_message>
<xml_diff>
--- a/horarios_optimizados-200-push_gap_0.80.xlsx
+++ b/horarios_optimizados-200-push_gap_0.80.xlsx
@@ -617,47 +617,19 @@
           <t>Lun</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="E5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J5" s="4" t="inlineStr"/>
+      <c r="B5" s="4" t="inlineStr"/>
+      <c r="C5" s="4" t="inlineStr"/>
+      <c r="D5" s="4" t="inlineStr"/>
+      <c r="E5" s="4" t="inlineStr"/>
+      <c r="F5" s="4" t="inlineStr"/>
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr"/>
+      <c r="I5" s="4" t="inlineStr"/>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="K5" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -673,45 +645,57 @@
           <t>R</t>
         </is>
       </c>
-      <c r="N5" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="O5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Q5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="T5" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="U5" s="4" t="inlineStr"/>
-      <c r="V5" s="4" t="inlineStr"/>
-      <c r="W5" s="4" t="inlineStr"/>
-      <c r="X5" s="4" t="inlineStr"/>
+      <c r="N5" s="4" t="inlineStr"/>
+      <c r="O5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="P5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="Q5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="R5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="S5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="T5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="U5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="W5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="X5" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -719,26 +703,102 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr"/>
-      <c r="C6" s="4" t="inlineStr"/>
-      <c r="D6" s="4" t="inlineStr"/>
-      <c r="E6" s="4" t="inlineStr"/>
-      <c r="F6" s="4" t="inlineStr"/>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="inlineStr"/>
-      <c r="I6" s="4" t="inlineStr"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="J6" s="4" t="inlineStr"/>
-      <c r="K6" s="4" t="inlineStr"/>
-      <c r="L6" s="4" t="inlineStr"/>
-      <c r="M6" s="4" t="inlineStr"/>
-      <c r="N6" s="4" t="inlineStr"/>
-      <c r="O6" s="4" t="inlineStr"/>
-      <c r="P6" s="4" t="inlineStr"/>
-      <c r="Q6" s="4" t="inlineStr"/>
-      <c r="R6" s="4" t="inlineStr"/>
-      <c r="S6" s="4" t="inlineStr"/>
-      <c r="T6" s="4" t="inlineStr"/>
-      <c r="U6" s="4" t="inlineStr"/>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="T6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="U6" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="V6" s="4" t="inlineStr"/>
       <c r="W6" s="4" t="inlineStr"/>
       <c r="X6" s="4" t="inlineStr"/>
@@ -749,27 +809,55 @@
           <t>Mie</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr"/>
-      <c r="C7" s="4" t="inlineStr"/>
-      <c r="D7" s="4" t="inlineStr"/>
-      <c r="E7" s="4" t="inlineStr"/>
-      <c r="F7" s="4" t="inlineStr"/>
-      <c r="G7" s="4" t="inlineStr"/>
-      <c r="H7" s="4" t="inlineStr"/>
-      <c r="I7" s="4" t="inlineStr"/>
-      <c r="J7" s="4" t="inlineStr"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="K7" s="4" t="inlineStr"/>
       <c r="L7" s="4" t="inlineStr"/>
-      <c r="M7" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N7" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="M7" s="4" t="inlineStr"/>
+      <c r="N7" s="4" t="inlineStr"/>
       <c r="O7" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -815,9 +903,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="X7" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
+      <c r="X7" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -827,60 +915,40 @@
           <t>Jue</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="E8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="I8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="B8" s="4" t="inlineStr"/>
+      <c r="C8" s="4" t="inlineStr"/>
+      <c r="D8" s="4" t="inlineStr"/>
+      <c r="E8" s="4" t="inlineStr"/>
+      <c r="F8" s="4" t="inlineStr"/>
+      <c r="G8" s="4" t="inlineStr"/>
+      <c r="H8" s="4" t="inlineStr"/>
+      <c r="I8" s="4" t="inlineStr"/>
       <c r="J8" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K8" s="4" t="inlineStr"/>
-      <c r="L8" s="4" t="inlineStr"/>
-      <c r="M8" s="4" t="inlineStr"/>
-      <c r="N8" s="4" t="inlineStr"/>
-      <c r="O8" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M8" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O8" s="4" t="inlineStr"/>
       <c r="P8" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -921,9 +989,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="X8" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
+      <c r="X8" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -940,8 +1008,16 @@
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" s="4" t="inlineStr"/>
       <c r="H9" s="4" t="inlineStr"/>
-      <c r="I9" s="4" t="inlineStr"/>
-      <c r="J9" s="4" t="inlineStr"/>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="K9" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -962,11 +1038,7 @@
           <t>R</t>
         </is>
       </c>
-      <c r="O9" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="O9" s="4" t="inlineStr"/>
       <c r="P9" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -977,7 +1049,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="R9" s="4" t="inlineStr"/>
+      <c r="R9" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="S9" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1019,27 +1095,19 @@
       <c r="C10" s="4" t="inlineStr"/>
       <c r="D10" s="4" t="inlineStr"/>
       <c r="E10" s="4" t="inlineStr"/>
-      <c r="F10" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G10" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H10" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="F10" s="4" t="inlineStr"/>
+      <c r="G10" s="4" t="inlineStr"/>
+      <c r="H10" s="4" t="inlineStr"/>
       <c r="I10" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J10" s="4" t="inlineStr"/>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="K10" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1060,11 +1128,7 @@
           <t>R</t>
         </is>
       </c>
-      <c r="O10" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="O10" s="4" t="inlineStr"/>
       <c r="P10" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1124,82 +1188,22 @@
       <c r="F11" s="4" t="inlineStr"/>
       <c r="G11" s="4" t="inlineStr"/>
       <c r="H11" s="4" t="inlineStr"/>
-      <c r="I11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="K11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="I11" s="4" t="inlineStr"/>
+      <c r="J11" s="4" t="inlineStr"/>
+      <c r="K11" s="4" t="inlineStr"/>
+      <c r="L11" s="4" t="inlineStr"/>
+      <c r="M11" s="4" t="inlineStr"/>
+      <c r="N11" s="4" t="inlineStr"/>
       <c r="O11" s="4" t="inlineStr"/>
-      <c r="P11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="Q11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="R11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="T11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="U11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="V11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="W11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="X11" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="P11" s="4" t="inlineStr"/>
+      <c r="Q11" s="4" t="inlineStr"/>
+      <c r="R11" s="4" t="inlineStr"/>
+      <c r="S11" s="4" t="inlineStr"/>
+      <c r="T11" s="4" t="inlineStr"/>
+      <c r="U11" s="4" t="inlineStr"/>
+      <c r="V11" s="4" t="inlineStr"/>
+      <c r="W11" s="4" t="inlineStr"/>
+      <c r="X11" s="4" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
@@ -1301,18 +1305,66 @@
       <c r="J15" s="4" t="inlineStr"/>
       <c r="K15" s="4" t="inlineStr"/>
       <c r="L15" s="4" t="inlineStr"/>
-      <c r="M15" s="4" t="inlineStr"/>
-      <c r="N15" s="4" t="inlineStr"/>
-      <c r="O15" s="4" t="inlineStr"/>
-      <c r="P15" s="4" t="inlineStr"/>
-      <c r="Q15" s="4" t="inlineStr"/>
-      <c r="R15" s="4" t="inlineStr"/>
-      <c r="S15" s="4" t="inlineStr"/>
-      <c r="T15" s="4" t="inlineStr"/>
-      <c r="U15" s="4" t="inlineStr"/>
-      <c r="V15" s="4" t="inlineStr"/>
-      <c r="W15" s="4" t="inlineStr"/>
-      <c r="X15" s="4" t="inlineStr"/>
+      <c r="M15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="P15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="Q15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="R15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="S15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="T15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="U15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="W15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="X15" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -1320,60 +1372,40 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="E16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="B16" s="4" t="inlineStr"/>
+      <c r="C16" s="4" t="inlineStr"/>
+      <c r="D16" s="4" t="inlineStr"/>
+      <c r="E16" s="4" t="inlineStr"/>
+      <c r="F16" s="4" t="inlineStr"/>
+      <c r="G16" s="4" t="inlineStr"/>
+      <c r="H16" s="4" t="inlineStr"/>
+      <c r="I16" s="4" t="inlineStr"/>
       <c r="J16" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K16" s="4" t="inlineStr"/>
-      <c r="L16" s="4" t="inlineStr"/>
-      <c r="M16" s="4" t="inlineStr"/>
-      <c r="N16" s="4" t="inlineStr"/>
-      <c r="O16" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="K16" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L16" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M16" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N16" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O16" s="4" t="inlineStr"/>
       <c r="P16" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1414,9 +1446,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="X16" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
+      <c r="X16" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -1464,11 +1496,7 @@
           <t>R</t>
         </is>
       </c>
-      <c r="P17" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="P17" s="4" t="inlineStr"/>
       <c r="Q17" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1479,7 +1507,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="S17" s="4" t="inlineStr"/>
+      <c r="S17" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="T17" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -1520,77 +1552,21 @@
       <c r="G18" s="4" t="inlineStr"/>
       <c r="H18" s="4" t="inlineStr"/>
       <c r="I18" s="4" t="inlineStr"/>
-      <c r="J18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="K18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="J18" s="4" t="inlineStr"/>
+      <c r="K18" s="4" t="inlineStr"/>
+      <c r="L18" s="4" t="inlineStr"/>
+      <c r="M18" s="4" t="inlineStr"/>
+      <c r="N18" s="4" t="inlineStr"/>
       <c r="O18" s="4" t="inlineStr"/>
-      <c r="P18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="Q18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="R18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="T18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="U18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="V18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="W18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="X18" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="P18" s="4" t="inlineStr"/>
+      <c r="Q18" s="4" t="inlineStr"/>
+      <c r="R18" s="4" t="inlineStr"/>
+      <c r="S18" s="4" t="inlineStr"/>
+      <c r="T18" s="4" t="inlineStr"/>
+      <c r="U18" s="4" t="inlineStr"/>
+      <c r="V18" s="4" t="inlineStr"/>
+      <c r="W18" s="4" t="inlineStr"/>
+      <c r="X18" s="4" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -1719,69 +1695,65 @@
           <t>R</t>
         </is>
       </c>
-      <c r="I20" s="4" t="inlineStr"/>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="J20" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K20" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L20" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M20" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N20" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="O20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Q20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="T20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="U20" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="V20" s="4" t="inlineStr"/>
-      <c r="W20" s="4" t="inlineStr"/>
+      <c r="K20" s="4" t="inlineStr"/>
+      <c r="L20" s="4" t="inlineStr"/>
+      <c r="M20" s="4" t="inlineStr"/>
+      <c r="N20" s="4" t="inlineStr"/>
+      <c r="O20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="P20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="Q20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="R20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="S20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="T20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="U20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="W20" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="X20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2015,65 +1987,37 @@
           <t>R</t>
         </is>
       </c>
-      <c r="J25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="K25" s="4" t="inlineStr"/>
-      <c r="L25" s="4" t="inlineStr"/>
-      <c r="M25" s="4" t="inlineStr"/>
-      <c r="N25" s="4" t="inlineStr"/>
-      <c r="O25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="P25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="Q25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="R25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="T25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="U25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="V25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="W25" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="X25" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="J25" s="4" t="inlineStr"/>
+      <c r="K25" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L25" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M25" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N25" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O25" s="4" t="inlineStr"/>
+      <c r="P25" s="4" t="inlineStr"/>
+      <c r="Q25" s="4" t="inlineStr"/>
+      <c r="R25" s="4" t="inlineStr"/>
+      <c r="S25" s="4" t="inlineStr"/>
+      <c r="T25" s="4" t="inlineStr"/>
+      <c r="U25" s="4" t="inlineStr"/>
+      <c r="V25" s="4" t="inlineStr"/>
+      <c r="W25" s="4" t="inlineStr"/>
+      <c r="X25" s="4" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
@@ -2081,102 +2025,26 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="E26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="F26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="I26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="B26" s="4" t="inlineStr"/>
+      <c r="C26" s="4" t="inlineStr"/>
+      <c r="D26" s="4" t="inlineStr"/>
+      <c r="E26" s="4" t="inlineStr"/>
+      <c r="F26" s="4" t="inlineStr"/>
+      <c r="G26" s="4" t="inlineStr"/>
+      <c r="H26" s="4" t="inlineStr"/>
+      <c r="I26" s="4" t="inlineStr"/>
       <c r="J26" s="4" t="inlineStr"/>
-      <c r="K26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N26" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="O26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="Q26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="T26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="U26" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="K26" s="4" t="inlineStr"/>
+      <c r="L26" s="4" t="inlineStr"/>
+      <c r="M26" s="4" t="inlineStr"/>
+      <c r="N26" s="4" t="inlineStr"/>
+      <c r="O26" s="4" t="inlineStr"/>
+      <c r="P26" s="4" t="inlineStr"/>
+      <c r="Q26" s="4" t="inlineStr"/>
+      <c r="R26" s="4" t="inlineStr"/>
+      <c r="S26" s="4" t="inlineStr"/>
+      <c r="T26" s="4" t="inlineStr"/>
+      <c r="U26" s="4" t="inlineStr"/>
       <c r="V26" s="4" t="inlineStr"/>
       <c r="W26" s="4" t="inlineStr"/>
       <c r="X26" s="4" t="inlineStr"/>
@@ -2227,28 +2095,40 @@
           <t>R</t>
         </is>
       </c>
-      <c r="J27" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="K27" s="4" t="inlineStr"/>
-      <c r="L27" s="4" t="inlineStr"/>
-      <c r="M27" s="4" t="inlineStr"/>
-      <c r="N27" s="4" t="inlineStr"/>
-      <c r="O27" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="P27" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="Q27" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
+      <c r="J27" s="4" t="inlineStr"/>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M27" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N27" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="O27" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P27" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q27" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
       <c r="R27" s="6" t="inlineStr">
@@ -2342,9 +2222,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="O28" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
+      <c r="O28" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
       <c r="P28" s="6" t="inlineStr">
@@ -2489,19 +2369,27 @@
       <c r="C30" s="4" t="inlineStr"/>
       <c r="D30" s="4" t="inlineStr"/>
       <c r="E30" s="4" t="inlineStr"/>
-      <c r="F30" s="4" t="inlineStr"/>
-      <c r="G30" s="4" t="inlineStr"/>
-      <c r="H30" s="4" t="inlineStr"/>
+      <c r="F30" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H30" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="I30" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="J30" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="J30" s="4" t="inlineStr"/>
       <c r="K30" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -2527,7 +2415,11 @@
           <t>R</t>
         </is>
       </c>
-      <c r="P30" s="4" t="inlineStr"/>
+      <c r="P30" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="Q30" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -2581,23 +2473,87 @@
       <c r="E31" s="4" t="inlineStr"/>
       <c r="F31" s="4" t="inlineStr"/>
       <c r="G31" s="4" t="inlineStr"/>
-      <c r="H31" s="4" t="inlineStr"/>
-      <c r="I31" s="4" t="inlineStr"/>
-      <c r="J31" s="4" t="inlineStr"/>
-      <c r="K31" s="4" t="inlineStr"/>
-      <c r="L31" s="4" t="inlineStr"/>
-      <c r="M31" s="4" t="inlineStr"/>
-      <c r="N31" s="4" t="inlineStr"/>
+      <c r="H31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="K31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="O31" s="4" t="inlineStr"/>
-      <c r="P31" s="4" t="inlineStr"/>
-      <c r="Q31" s="4" t="inlineStr"/>
-      <c r="R31" s="4" t="inlineStr"/>
-      <c r="S31" s="4" t="inlineStr"/>
-      <c r="T31" s="4" t="inlineStr"/>
-      <c r="U31" s="4" t="inlineStr"/>
-      <c r="V31" s="4" t="inlineStr"/>
-      <c r="W31" s="4" t="inlineStr"/>
-      <c r="X31" s="4" t="inlineStr"/>
+      <c r="P31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="Q31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="R31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="S31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="T31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="U31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="W31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="X31" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
@@ -2688,40 +2644,60 @@
           <t>Lun</t>
         </is>
       </c>
-      <c r="B35" s="4" t="inlineStr"/>
-      <c r="C35" s="4" t="inlineStr"/>
-      <c r="D35" s="4" t="inlineStr"/>
-      <c r="E35" s="4" t="inlineStr"/>
-      <c r="F35" s="4" t="inlineStr"/>
-      <c r="G35" s="4" t="inlineStr"/>
-      <c r="H35" s="4" t="inlineStr"/>
-      <c r="I35" s="4" t="inlineStr"/>
+      <c r="B35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="F35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="J35" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="O35" s="4" t="inlineStr"/>
+      <c r="K35" s="4" t="inlineStr"/>
+      <c r="L35" s="4" t="inlineStr"/>
+      <c r="M35" s="4" t="inlineStr"/>
+      <c r="N35" s="4" t="inlineStr"/>
+      <c r="O35" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="P35" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -2732,41 +2708,25 @@
           <t>R</t>
         </is>
       </c>
-      <c r="R35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="T35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="U35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="V35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="W35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="X35" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="R35" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S35" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="T35" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="U35" s="4" t="inlineStr"/>
+      <c r="V35" s="4" t="inlineStr"/>
+      <c r="W35" s="4" t="inlineStr"/>
+      <c r="X35" s="4" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
@@ -2774,40 +2734,60 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B36" s="4" t="inlineStr"/>
-      <c r="C36" s="4" t="inlineStr"/>
-      <c r="D36" s="4" t="inlineStr"/>
-      <c r="E36" s="4" t="inlineStr"/>
-      <c r="F36" s="4" t="inlineStr"/>
-      <c r="G36" s="4" t="inlineStr"/>
-      <c r="H36" s="4" t="inlineStr"/>
-      <c r="I36" s="4" t="inlineStr"/>
+      <c r="B36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="F36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="J36" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K36" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L36" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M36" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N36" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="O36" s="4" t="inlineStr"/>
+      <c r="K36" s="4" t="inlineStr"/>
+      <c r="L36" s="4" t="inlineStr"/>
+      <c r="M36" s="4" t="inlineStr"/>
+      <c r="N36" s="4" t="inlineStr"/>
+      <c r="O36" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="P36" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -2848,9 +2828,9 @@
           <t>R</t>
         </is>
       </c>
-      <c r="X36" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
+      <c r="X36" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
     </row>
@@ -2860,67 +2840,19 @@
           <t>Mie</t>
         </is>
       </c>
-      <c r="B37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="C37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="D37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="E37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="F37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="G37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="H37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="I37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="B37" s="4" t="inlineStr"/>
+      <c r="C37" s="4" t="inlineStr"/>
+      <c r="D37" s="4" t="inlineStr"/>
+      <c r="E37" s="4" t="inlineStr"/>
+      <c r="F37" s="4" t="inlineStr"/>
+      <c r="G37" s="4" t="inlineStr"/>
+      <c r="H37" s="4" t="inlineStr"/>
+      <c r="I37" s="4" t="inlineStr"/>
       <c r="J37" s="4" t="inlineStr"/>
-      <c r="K37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="L37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="M37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="N37" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="K37" s="4" t="inlineStr"/>
+      <c r="L37" s="4" t="inlineStr"/>
+      <c r="M37" s="4" t="inlineStr"/>
+      <c r="N37" s="4" t="inlineStr"/>
       <c r="O37" s="4" t="inlineStr"/>
       <c r="P37" s="4" t="inlineStr"/>
       <c r="Q37" s="4" t="inlineStr"/>
@@ -2938,29 +2870,105 @@
           <t>Jue</t>
         </is>
       </c>
-      <c r="B38" s="4" t="inlineStr"/>
-      <c r="C38" s="4" t="inlineStr"/>
-      <c r="D38" s="4" t="inlineStr"/>
-      <c r="E38" s="4" t="inlineStr"/>
-      <c r="F38" s="4" t="inlineStr"/>
-      <c r="G38" s="4" t="inlineStr"/>
-      <c r="H38" s="4" t="inlineStr"/>
-      <c r="I38" s="4" t="inlineStr"/>
-      <c r="J38" s="4" t="inlineStr"/>
+      <c r="B38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="E38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="F38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="H38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="J38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="K38" s="4" t="inlineStr"/>
       <c r="L38" s="4" t="inlineStr"/>
       <c r="M38" s="4" t="inlineStr"/>
       <c r="N38" s="4" t="inlineStr"/>
-      <c r="O38" s="4" t="inlineStr"/>
-      <c r="P38" s="4" t="inlineStr"/>
-      <c r="Q38" s="4" t="inlineStr"/>
-      <c r="R38" s="4" t="inlineStr"/>
-      <c r="S38" s="4" t="inlineStr"/>
-      <c r="T38" s="4" t="inlineStr"/>
-      <c r="U38" s="4" t="inlineStr"/>
-      <c r="V38" s="4" t="inlineStr"/>
-      <c r="W38" s="4" t="inlineStr"/>
-      <c r="X38" s="4" t="inlineStr"/>
+      <c r="O38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="P38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="Q38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="R38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="S38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="T38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="U38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="V38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="W38" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="X38" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -2975,16 +2983,8 @@
       <c r="F39" s="4" t="inlineStr"/>
       <c r="G39" s="4" t="inlineStr"/>
       <c r="H39" s="4" t="inlineStr"/>
-      <c r="I39" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="J39" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="I39" s="4" t="inlineStr"/>
+      <c r="J39" s="4" t="inlineStr"/>
       <c r="K39" s="5" t="inlineStr">
         <is>
           <t>R</t>
@@ -3093,65 +3093,69 @@
           <t>R</t>
         </is>
       </c>
-      <c r="I40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="I40" s="4" t="inlineStr"/>
       <c r="J40" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="K40" s="4" t="inlineStr"/>
-      <c r="L40" s="4" t="inlineStr"/>
-      <c r="M40" s="4" t="inlineStr"/>
-      <c r="N40" s="4" t="inlineStr"/>
+      <c r="K40" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="L40" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="M40" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="N40" s="5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
       <c r="O40" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="P40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="Q40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="R40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="S40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="T40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="U40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="V40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="W40" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="P40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="S40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="T40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="U40" s="6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="V40" s="4" t="inlineStr"/>
+      <c r="W40" s="4" t="inlineStr"/>
       <c r="X40" s="4" t="inlineStr"/>
     </row>
     <row r="41">
@@ -3186,11 +3190,7 @@
           <t>R</t>
         </is>
       </c>
-      <c r="H41" s="5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
+      <c r="H41" s="4" t="inlineStr"/>
       <c r="I41" s="4" t="inlineStr"/>
       <c r="J41" s="4" t="inlineStr"/>
       <c r="K41" s="5" t="inlineStr">
@@ -3346,26 +3346,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I2" t="n">
         <v>0.5</v>
@@ -3389,17 +3389,29 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Descanso</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4">
@@ -3420,20 +3432,30 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14:30</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>6</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+        <v>9.5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3453,17 +3475,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -3472,10 +3494,10 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -3496,17 +3518,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -3515,7 +3537,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="I6" t="n">
         <v>0.5</v>
@@ -3539,17 +3561,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -3558,7 +3580,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="I7" t="n">
         <v>0.5</v>
@@ -3582,29 +3604,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12:30</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
+          <t>Descanso</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3625,18 +3635,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Descanso</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3656,17 +3668,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>09:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -3675,10 +3687,10 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11">
@@ -3704,12 +3716,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -3742,29 +3754,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
+          <t>Descanso</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3833,24 +3833,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -3919,24 +3919,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>13:30</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
       <c r="H16" t="n">
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17">
@@ -3957,29 +3957,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>13:30</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>19:00</t>
-        </is>
-      </c>
+          <t>Descanso</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>9.5</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -4005,24 +3993,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>13:30</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19">
@@ -4129,17 +4117,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -4148,7 +4136,7 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="I21" t="n">
         <v>0.5</v>
@@ -4172,17 +4160,29 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Descanso</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23">
@@ -4203,29 +4203,29 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -4246,29 +4246,29 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="I24" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -4289,29 +4289,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>09:00</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>13:00</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>13:30</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>15:30</t>
-        </is>
-      </c>
+          <t>Descanso</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -4332,17 +4320,29 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Descanso</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -4363,7 +4363,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="I27" t="n">
         <v>0.5</v>
@@ -4411,24 +4411,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>12:30</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -4468,10 +4468,10 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>